<commit_message>
marked ANOVA passed on List_of_Cells_from_Ed.xlsx
</commit_message>
<xml_diff>
--- a/resources/List_of_Cells_from_Ed.xlsx
+++ b/resources/List_of_Cells_from_Ed.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="70">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -224,6 +225,12 @@
   </si>
   <si>
     <t xml:space="preserve">same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of regression plots with &lt; 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA passed highlighted</t>
   </si>
 </sst>
 </file>
@@ -234,7 +241,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -262,18 +269,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -317,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,11 +346,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,11 +397,11 @@
   </sheetPr>
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C118" activeCellId="0" sqref="C118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.66"/>
@@ -705,7 +737,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -725,7 +757,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -745,7 +777,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -785,7 +817,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -805,7 +837,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -825,7 +857,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -865,7 +897,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B25" s="0" t="n">
@@ -885,7 +917,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B26" s="0" t="n">
@@ -905,7 +937,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -945,7 +977,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B29" s="0" t="n">
@@ -965,7 +997,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B30" s="0" t="n">
@@ -985,7 +1017,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B31" s="0" t="n">
@@ -1025,7 +1057,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -1045,7 +1077,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -1065,7 +1097,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -1145,7 +1177,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="n">
+      <c r="A39" s="5" t="n">
         <v>45208</v>
       </c>
       <c r="B39" s="0" t="n">
@@ -1168,7 +1200,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="n">
+      <c r="A40" s="5" t="n">
         <v>45208</v>
       </c>
       <c r="B40" s="0" t="n">
@@ -1191,7 +1223,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="n">
+      <c r="A41" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B41" s="0" t="n">
@@ -1211,7 +1243,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="n">
+      <c r="A42" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B42" s="0" t="n">
@@ -1231,7 +1263,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="n">
+      <c r="A43" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B43" s="0" t="n">
@@ -1254,7 +1286,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="n">
+      <c r="A44" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B44" s="0" t="n">
@@ -1274,7 +1306,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="n">
+      <c r="A45" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B45" s="0" t="n">
@@ -1294,7 +1326,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="n">
+      <c r="A46" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B46" s="0" t="n">
@@ -1314,7 +1346,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="n">
+      <c r="A47" s="5" t="n">
         <v>45209</v>
       </c>
       <c r="B47" s="0" t="n">
@@ -1334,7 +1366,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="n">
+      <c r="A48" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B48" s="0" t="n">
@@ -1354,7 +1386,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="n">
+      <c r="A49" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B49" s="0" t="n">
@@ -1374,7 +1406,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="n">
+      <c r="A50" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B50" s="0" t="n">
@@ -1394,7 +1426,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="n">
+      <c r="A51" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B51" s="0" t="n">
@@ -1417,7 +1449,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="n">
+      <c r="A52" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B52" s="0" t="n">
@@ -1437,7 +1469,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="n">
+      <c r="A53" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B53" s="0" t="n">
@@ -1460,7 +1492,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="n">
+      <c r="A54" s="5" t="n">
         <v>45210</v>
       </c>
       <c r="B54" s="0" t="n">
@@ -1483,7 +1515,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="n">
+      <c r="A55" s="5" t="n">
         <v>45223</v>
       </c>
       <c r="B55" s="0" t="n">
@@ -1503,7 +1535,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="n">
+      <c r="A56" s="5" t="n">
         <v>45223</v>
       </c>
       <c r="B56" s="0" t="n">
@@ -1526,7 +1558,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="n">
+      <c r="A57" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B57" s="0" t="n">
@@ -1552,7 +1584,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="n">
+      <c r="A58" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B58" s="0" t="n">
@@ -1578,7 +1610,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="n">
+      <c r="A59" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B59" s="0" t="n">
@@ -1604,7 +1636,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="n">
+      <c r="A60" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B60" s="0" t="n">
@@ -1624,7 +1656,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6" t="n">
+      <c r="A61" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B61" s="0" t="n">
@@ -1644,7 +1676,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6" t="n">
+      <c r="A62" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B62" s="0" t="n">
@@ -1664,7 +1696,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="6" t="n">
+      <c r="A63" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B63" s="0" t="n">
@@ -1684,7 +1716,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6" t="n">
+      <c r="A64" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B64" s="0" t="n">
@@ -1704,7 +1736,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="6" t="n">
+      <c r="A65" s="5" t="n">
         <v>45226</v>
       </c>
       <c r="B65" s="0" t="n">
@@ -1727,7 +1759,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6" t="n">
+      <c r="A66" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B66" s="0" t="n">
@@ -1747,7 +1779,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="n">
+      <c r="A67" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B67" s="0" t="n">
@@ -1767,7 +1799,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="n">
+      <c r="A68" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B68" s="0" t="n">
@@ -1787,7 +1819,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="n">
+      <c r="A69" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B69" s="0" t="n">
@@ -1810,7 +1842,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="n">
+      <c r="A70" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B70" s="0" t="n">
@@ -1830,7 +1862,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="n">
+      <c r="A71" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B71" s="0" t="n">
@@ -1850,7 +1882,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6" t="n">
+      <c r="A72" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B72" s="0" t="n">
@@ -1873,7 +1905,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6" t="n">
+      <c r="A73" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B73" s="0" t="n">
@@ -1893,7 +1925,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6" t="n">
+      <c r="A74" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B74" s="0" t="n">
@@ -1913,7 +1945,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="6" t="n">
+      <c r="A75" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B75" s="0" t="n">
@@ -1933,7 +1965,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="6" t="n">
+      <c r="A76" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B76" s="0" t="n">
@@ -1953,7 +1985,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6" t="n">
+      <c r="A77" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B77" s="0" t="n">
@@ -1973,7 +2005,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6" t="n">
+      <c r="A78" s="5" t="n">
         <v>45230</v>
       </c>
       <c r="B78" s="0" t="n">
@@ -1996,7 +2028,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6" t="n">
+      <c r="A79" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B79" s="0" t="n">
@@ -2016,7 +2048,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6" t="n">
+      <c r="A80" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B80" s="0" t="n">
@@ -2039,7 +2071,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="6" t="n">
+      <c r="A81" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B81" s="0" t="n">
@@ -2059,7 +2091,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="6" t="n">
+      <c r="A82" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B82" s="0" t="n">
@@ -2079,7 +2111,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="6" t="n">
+      <c r="A83" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B83" s="0" t="n">
@@ -2099,7 +2131,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="6" t="n">
+      <c r="A84" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B84" s="0" t="n">
@@ -2119,7 +2151,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="6" t="n">
+      <c r="A85" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B85" s="0" t="n">
@@ -2139,7 +2171,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="6" t="n">
+      <c r="A86" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B86" s="0" t="n">
@@ -2162,7 +2194,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="6" t="n">
+      <c r="A87" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B87" s="0" t="n">
@@ -2182,7 +2214,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="6" t="n">
+      <c r="A88" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B88" s="0" t="n">
@@ -2202,7 +2234,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="6" t="n">
+      <c r="A89" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B89" s="0" t="n">
@@ -2222,7 +2254,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="6" t="n">
+      <c r="A90" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B90" s="0" t="n">
@@ -2242,7 +2274,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="6" t="n">
+      <c r="A91" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B91" s="0" t="n">
@@ -2262,7 +2294,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="6" t="n">
+      <c r="A92" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B92" s="0" t="n">
@@ -2282,7 +2314,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="6" t="n">
+      <c r="A93" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B93" s="0" t="n">
@@ -2302,7 +2334,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="6" t="n">
+      <c r="A94" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B94" s="0" t="n">
@@ -2322,7 +2354,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="6" t="n">
+      <c r="A95" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B95" s="0" t="n">
@@ -2342,7 +2374,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="6" t="n">
+      <c r="A96" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="B96" s="0" t="n">
@@ -2362,7 +2394,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="6" t="n">
+      <c r="A97" s="5" t="n">
         <v>45241</v>
       </c>
       <c r="B97" s="0" t="n">
@@ -2382,7 +2414,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="6" t="n">
+      <c r="A98" s="5" t="n">
         <v>45241</v>
       </c>
       <c r="B98" s="0" t="n">
@@ -2402,7 +2434,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="6" t="n">
+      <c r="A99" s="5" t="n">
         <v>45241</v>
       </c>
       <c r="B99" s="0" t="n">
@@ -2422,7 +2454,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="6" t="n">
+      <c r="A100" s="5" t="n">
         <v>45242</v>
       </c>
       <c r="B100" s="0" t="n">
@@ -2445,7 +2477,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="6" t="n">
+      <c r="A101" s="5" t="n">
         <v>45250</v>
       </c>
       <c r="B101" s="0" t="n">
@@ -2465,7 +2497,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="6" t="n">
+      <c r="A102" s="5" t="n">
         <v>45252</v>
       </c>
       <c r="B102" s="0" t="n">
@@ -2488,7 +2520,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="6" t="n">
+      <c r="A103" s="5" t="n">
         <v>45252</v>
       </c>
       <c r="B103" s="0" t="n">
@@ -2508,7 +2540,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="6" t="n">
+      <c r="A104" s="5" t="n">
         <v>45255</v>
       </c>
       <c r="B104" s="0" t="n">
@@ -2528,7 +2560,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="6" t="n">
+      <c r="A105" s="5" t="n">
         <v>45255</v>
       </c>
       <c r="B105" s="0" t="n">
@@ -2548,7 +2580,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="6" t="n">
+      <c r="A106" s="5" t="n">
         <v>45255</v>
       </c>
       <c r="B106" s="0" t="n">
@@ -2568,7 +2600,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="6" t="n">
+      <c r="A107" s="5" t="n">
         <v>45255</v>
       </c>
       <c r="B107" s="0" t="n">
@@ -2588,7 +2620,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="6" t="n">
+      <c r="A108" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B108" s="0" t="n">
@@ -2611,7 +2643,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="6" t="n">
+      <c r="A109" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B109" s="0" t="n">
@@ -2631,7 +2663,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="6" t="n">
+      <c r="A110" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B110" s="0" t="n">
@@ -2651,7 +2683,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="6" t="n">
+      <c r="A111" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B111" s="0" t="n">
@@ -2674,7 +2706,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="6" t="n">
+      <c r="A112" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B112" s="0" t="n">
@@ -2694,7 +2726,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="6" t="n">
+      <c r="A113" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B113" s="0" t="n">
@@ -2717,7 +2749,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="6" t="n">
+      <c r="A114" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B114" s="0" t="n">
@@ -2737,7 +2769,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="6" t="n">
+      <c r="A115" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B115" s="0" t="n">
@@ -2757,7 +2789,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="6" t="n">
+      <c r="A116" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B116" s="0" t="n">
@@ -2780,7 +2812,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="6" t="n">
+      <c r="A117" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B117" s="0" t="n">
@@ -2800,7 +2832,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="6" t="n">
+      <c r="A118" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B118" s="0" t="n">
@@ -2823,7 +2855,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="6" t="n">
+      <c r="A119" s="5" t="n">
         <v>45258</v>
       </c>
       <c r="B119" s="0" t="n">
@@ -2846,7 +2878,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="6" t="n">
+      <c r="A120" s="5" t="n">
         <v>45265</v>
       </c>
       <c r="B120" s="0" t="n">
@@ -2869,7 +2901,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="6" t="n">
+      <c r="A121" s="5" t="n">
         <v>45265</v>
       </c>
       <c r="B121" s="0" t="n">
@@ -2892,7 +2924,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="6" t="n">
+      <c r="A122" s="5" t="n">
         <v>45265</v>
       </c>
       <c r="B122" s="0" t="n">
@@ -2915,7 +2947,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="6"/>
+      <c r="A152" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2926,4 +2958,2256 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I108"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="H1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>300</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>650</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>200</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <v>600</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>200</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>600</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>700</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E18" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E20" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B24" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B25" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B27" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B28" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="11" t="n">
+        <v>700</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B33" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11" t="n">
+        <v>750</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>250</v>
+      </c>
+      <c r="E35" s="11" t="n">
+        <v>750</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B36" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B47" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E47" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="12" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B49" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="12" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B51" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H51" s="11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="12" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B53" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="11" t="n">
+        <v>250</v>
+      </c>
+      <c r="E53" s="11" t="n">
+        <v>750</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="12" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B56" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="11" t="n">
+        <v>750</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="12" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B58" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="11" t="n">
+        <v>750</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H58" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="12" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B60" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="11" t="n">
+        <v>250</v>
+      </c>
+      <c r="E60" s="11" t="n">
+        <v>600</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H60" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="12" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B62" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E62" s="11" t="n">
+        <v>600</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H62" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="12" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B70" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E70" s="11" t="n">
+        <v>700</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H70" s="11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1750</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="5" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="5" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="5" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="5" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="5" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="5" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="5" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H108" s="0" t="n">
+        <f aca="false">SUM(H2:H70)</f>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>